<commit_message>
Feat[FE_Stats_Note]: Linde stats code
</commit_message>
<xml_diff>
--- a/Data/FE_Stats_Spreadsheets.xlsx
+++ b/Data/FE_Stats_Spreadsheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trim\Documents\Code Projects\Python\FE Stats Classifier\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trim\VS Code Projects\Python\FE Stats Classifier\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70608D8-8969-4098-8A6A-EB2F5086BE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7288F73B-DF2A-4C25-B641-02E3A55AA7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="14265" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{0D99ECB4-B56B-4732-8632-B82B2C74A840}"/>
+    <workbookView xWindow="16080" yWindow="14265" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{0D99ECB4-B56B-4732-8632-B82B2C74A840}"/>
   </bookViews>
   <sheets>
     <sheet name="Marth Stats" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13EBB89-714B-4E07-9BB1-2F3109D286E4}">
   <dimension ref="B2:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2491,8 +2491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65FF1B8-4E3E-489B-8FF1-706C20CFF46F}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54:I56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Feat[FE_Stats_Note]: Palla stats analysis
</commit_message>
<xml_diff>
--- a/Data/FE_Stats_Spreadsheets.xlsx
+++ b/Data/FE_Stats_Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trim\VS Code Projects\Python\FE Stats Classifier\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7288F73B-DF2A-4C25-B641-02E3A55AA7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D5D9B-523D-41E8-A1E9-602EA3121870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="14265" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{0D99ECB4-B56B-4732-8632-B82B2C74A840}"/>
+    <workbookView xWindow="16080" yWindow="14265" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{0D99ECB4-B56B-4732-8632-B82B2C74A840}"/>
   </bookViews>
   <sheets>
     <sheet name="Marth Stats" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13EBB89-714B-4E07-9BB1-2F3109D286E4}">
   <dimension ref="B2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1325,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C79018-788B-4FF2-BBF8-742A97FD6E9E}">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>